<commit_message>
added timings and updated interactions
</commit_message>
<xml_diff>
--- a/study/timings.xlsx.xlsx
+++ b/study/timings.xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlong/Documents/Github/sat-map/study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06375FF-DFA5-6049-ACEC-CA16EE67C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1D2062-A270-2349-8072-647CE03CB5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="12800" yWindow="520" windowWidth="25600" windowHeight="26220" xr2:uid="{3BFC56D9-92D8-DF43-8DB0-3445DA5A4414}"/>
+    <workbookView xWindow="3760" yWindow="500" windowWidth="28340" windowHeight="19840" xr2:uid="{3BFC56D9-92D8-DF43-8DB0-3445DA5A4414}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>p q</t>
+  </si>
+  <si>
+    <t>James P</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,6 +524,9 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -554,6 +560,9 @@
       <c r="B8" t="s">
         <v>4</v>
       </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -608,6 +617,12 @@
         <f>A12+TIME(0,10,0)</f>
         <v>0.53472222222222199</v>
       </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>

</xml_diff>